<commit_message>
add median in a excel file
</commit_message>
<xml_diff>
--- a/r_stat.xlsx
+++ b/r_stat.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Research Project\mental account\Tickers-Bloomberg\Ticker_moderate_US\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>r_bond.mean</t>
   </si>
@@ -194,12 +199,16 @@
   </si>
   <si>
     <t>WMBLX</t>
+  </si>
+  <si>
+    <t>Median</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0000_ "/>
   </numFmts>
@@ -235,7 +244,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -258,16 +267,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -277,6 +300,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -325,7 +351,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -358,9 +384,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -393,6 +436,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -568,21 +628,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E56"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -599,7 +659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -616,7 +676,7 @@
         <v>0.17069403905363881</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -633,7 +693,7 @@
         <v>55.27507728058724</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -650,7 +710,7 @@
         <v>0.43035655002538498</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -667,7 +727,7 @@
         <v>1.0391764070635761</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -684,7 +744,7 @@
         <v>0.15570268747157279</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -701,7 +761,7 @@
         <v>0.10320245140718221</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -718,7 +778,7 @@
         <v>0.13154497334889251</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -735,7 +795,7 @@
         <v>0.14545839782284681</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -752,7 +812,7 @@
         <v>0.14570869589981411</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -769,7 +829,7 @@
         <v>0.21207536694008211</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -786,7 +846,7 @@
         <v>0.11201674483158321</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -803,7 +863,7 @@
         <v>0.1352768231593201</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -820,7 +880,7 @@
         <v>0.1489690424273406</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -837,7 +897,7 @@
         <v>0.2437442584183146</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -854,7 +914,7 @@
         <v>0.12782338605512961</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -871,7 +931,7 @@
         <v>0.13372253048870111</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -888,7 +948,7 @@
         <v>0.13250281361643529</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -905,7 +965,7 @@
         <v>0.1184563884538601</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -922,7 +982,7 @@
         <v>0.13959160543202709</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -939,7 +999,7 @@
         <v>0.16152648525804511</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -956,7 +1016,7 @@
         <v>0.14307220445709701</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -973,7 +1033,7 @@
         <v>0.1409981121248704</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -990,7 +1050,7 @@
         <v>0.13024387808707391</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -1007,7 +1067,7 @@
         <v>0.14485450221054341</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -1024,7 +1084,7 @@
         <v>0.13345437070342869</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -1041,7 +1101,7 @@
         <v>0.15646015165207541</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -1058,7 +1118,7 @@
         <v>0.1074932245722182</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -1075,7 +1135,7 @@
         <v>0.13318432989681739</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
@@ -1092,7 +1152,7 @@
         <v>0.13878060344165291</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
@@ -1109,7 +1169,7 @@
         <v>0.15774399230478231</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
@@ -1126,7 +1186,7 @@
         <v>0.1270082571579795</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
@@ -1143,7 +1203,7 @@
         <v>0.16338764285410551</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -1160,7 +1220,7 @@
         <v>0.13608343538806289</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
@@ -1177,7 +1237,7 @@
         <v>0.1319565280215346</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -1194,7 +1254,7 @@
         <v>0.13708612894554581</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -1211,7 +1271,7 @@
         <v>0.1019921036914917</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -1228,7 +1288,7 @@
         <v>0.1245421240198385</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>42</v>
       </c>
@@ -1245,7 +1305,7 @@
         <v>0.16006414036360181</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>43</v>
       </c>
@@ -1262,7 +1322,7 @@
         <v>0.118572229372126</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
@@ -1279,7 +1339,7 @@
         <v>0.13749811554499769</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>45</v>
       </c>
@@ -1296,7 +1356,7 @@
         <v>0.1365885712798883</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
@@ -1313,7 +1373,7 @@
         <v>0.17271638837606679</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>47</v>
       </c>
@@ -1330,7 +1390,7 @@
         <v>1.0704132742565471</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>48</v>
       </c>
@@ -1347,7 +1407,7 @@
         <v>0.13568047533866301</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>49</v>
       </c>
@@ -1364,7 +1424,7 @@
         <v>0.17382570915268131</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>50</v>
       </c>
@@ -1381,7 +1441,7 @@
         <v>0.1179563589241038</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>51</v>
       </c>
@@ -1398,7 +1458,7 @@
         <v>0.16757283146881119</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
@@ -1415,7 +1475,7 @@
         <v>0.1170799943694589</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>53</v>
       </c>
@@ -1432,7 +1492,7 @@
         <v>0.13199389508299419</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
@@ -1449,7 +1509,7 @@
         <v>0.2522069148737498</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>55</v>
       </c>
@@ -1466,7 +1526,7 @@
         <v>0.20004512858530621</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
         <v>56</v>
       </c>
@@ -1483,7 +1543,7 @@
         <v>0.16526526377624581</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>57</v>
       </c>
@@ -1500,7 +1560,7 @@
         <v>0.1202749788131281</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>58</v>
       </c>
@@ -1517,7 +1577,7 @@
         <v>0.13849753261075359</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
@@ -1532,6 +1592,27 @@
       </c>
       <c r="E56" s="2">
         <v>0.12565845691865921</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A57" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="2">
+        <f>MEDIAN(B2:B56)</f>
+        <v>1.7695480305048202E-2</v>
+      </c>
+      <c r="C57" s="2">
+        <f t="shared" ref="C57:E57" si="0">MEDIAN(C2:C56)</f>
+        <v>3.1461777617472042E-2</v>
+      </c>
+      <c r="D57" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1176092269500531</v>
+      </c>
+      <c r="E57" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13849753261075359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>